<commit_message>
started drafting outline for narrative and coding regression tables inspired by Achen and Bartels
</commit_message>
<xml_diff>
--- a/data/state_populations.xlsx
+++ b/data/state_populations.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaylamanning/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Shared\ESTIMATES\V2019\Team Specific Material\Dissemination\Products\DISS\National-State-Commonwealth Totals\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE67BA1C-03CA-E14C-87C0-1A962800B949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37520" yWindow="2860" windowWidth="20180" windowHeight="12400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="720" yWindow="270" windowWidth="11100" windowHeight="5325"/>
   </bookViews>
   <sheets>
     <sheet name="NST01" sheetId="1" r:id="rId1"/>
@@ -744,11 +743,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1196,23 +1195,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1248,23 +1230,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1440,7 +1405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M67"/>
   <sheetViews>
@@ -1449,14 +1414,14 @@
       <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="13" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="13" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="2.25" customHeight="1">
+    <row r="1" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
@@ -1473,7 +1438,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
     </row>
-    <row r="2" spans="1:13" ht="25.5" customHeight="1">
+    <row r="2" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1455,7 @@
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1">
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
@@ -1511,7 +1476,7 @@
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -1550,7 +1515,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1556,7 @@
         <v>328239523</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1597,7 @@
         <v>55982803</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1673,7 +1638,7 @@
         <v>68329004</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +1679,7 @@
         <v>125580448</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -1755,7 +1720,7 @@
         <v>78347268</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -1796,7 +1761,7 @@
         <v>4903185</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1837,7 +1802,7 @@
         <v>731545</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1843,7 @@
         <v>7278717</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1919,7 +1884,7 @@
         <v>3017804</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>16</v>
       </c>
@@ -1960,7 +1925,7 @@
         <v>39512223</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
@@ -2001,7 +1966,7 @@
         <v>5758736</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
@@ -2042,7 +2007,7 @@
         <v>3565287</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
@@ -2083,7 +2048,7 @@
         <v>973764</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>20</v>
       </c>
@@ -2124,7 +2089,7 @@
         <v>705749</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>21</v>
       </c>
@@ -2165,7 +2130,7 @@
         <v>21477737</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
@@ -2206,7 +2171,7 @@
         <v>10617423</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>23</v>
       </c>
@@ -2247,7 +2212,7 @@
         <v>1415872</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>24</v>
       </c>
@@ -2288,7 +2253,7 @@
         <v>1787065</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>25</v>
       </c>
@@ -2329,7 +2294,7 @@
         <v>12671821</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>26</v>
       </c>
@@ -2370,7 +2335,7 @@
         <v>6732219</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>27</v>
       </c>
@@ -2411,7 +2376,7 @@
         <v>3155070</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>28</v>
       </c>
@@ -2452,7 +2417,7 @@
         <v>2913314</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
@@ -2493,7 +2458,7 @@
         <v>4467673</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>30</v>
       </c>
@@ -2534,7 +2499,7 @@
         <v>4648794</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>31</v>
       </c>
@@ -2575,7 +2540,7 @@
         <v>1344212</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>32</v>
       </c>
@@ -2616,7 +2581,7 @@
         <v>6045680</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>33</v>
       </c>
@@ -2657,7 +2622,7 @@
         <v>6892503</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>34</v>
       </c>
@@ -2698,7 +2663,7 @@
         <v>9986857</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>35</v>
       </c>
@@ -2739,7 +2704,7 @@
         <v>5639632</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>36</v>
       </c>
@@ -2780,7 +2745,7 @@
         <v>2976149</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>37</v>
       </c>
@@ -2821,7 +2786,7 @@
         <v>6137428</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>38</v>
       </c>
@@ -2862,7 +2827,7 @@
         <v>1068778</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>39</v>
       </c>
@@ -2903,7 +2868,7 @@
         <v>1934408</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>40</v>
       </c>
@@ -2944,7 +2909,7 @@
         <v>3080156</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>41</v>
       </c>
@@ -2985,7 +2950,7 @@
         <v>1359711</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>42</v>
       </c>
@@ -3026,7 +2991,7 @@
         <v>8882190</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>43</v>
       </c>
@@ -3067,7 +3032,7 @@
         <v>2096829</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>44</v>
       </c>
@@ -3108,7 +3073,7 @@
         <v>19453561</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>45</v>
       </c>
@@ -3149,7 +3114,7 @@
         <v>10488084</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>46</v>
       </c>
@@ -3190,7 +3155,7 @@
         <v>762062</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>47</v>
       </c>
@@ -3231,7 +3196,7 @@
         <v>11689100</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>48</v>
       </c>
@@ -3272,7 +3237,7 @@
         <v>3956971</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>49</v>
       </c>
@@ -3313,7 +3278,7 @@
         <v>4217737</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>50</v>
       </c>
@@ -3354,7 +3319,7 @@
         <v>12801989</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>51</v>
       </c>
@@ -3395,7 +3360,7 @@
         <v>1059361</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>52</v>
       </c>
@@ -3436,7 +3401,7 @@
         <v>5148714</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>53</v>
       </c>
@@ -3477,7 +3442,7 @@
         <v>884659</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>54</v>
       </c>
@@ -3518,7 +3483,7 @@
         <v>6829174</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>55</v>
       </c>
@@ -3559,7 +3524,7 @@
         <v>28995881</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>56</v>
       </c>
@@ -3600,7 +3565,7 @@
         <v>3205958</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>57</v>
       </c>
@@ -3641,7 +3606,7 @@
         <v>623989</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>58</v>
       </c>
@@ -3682,7 +3647,7 @@
         <v>8535519</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>59</v>
       </c>
@@ -3723,7 +3688,7 @@
         <v>7614893</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>60</v>
       </c>
@@ -3764,7 +3729,7 @@
         <v>1792147</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>61</v>
       </c>
@@ -3805,7 +3770,7 @@
         <v>5822434</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>62</v>
       </c>
@@ -3846,7 +3811,7 @@
         <v>578759</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -3861,7 +3826,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>5</v>
       </c>
@@ -3902,7 +3867,7 @@
         <v>3193694</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="36" customHeight="1">
+    <row r="63" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>63</v>
       </c>
@@ -3919,7 +3884,7 @@
       <c r="L63" s="31"/>
       <c r="M63" s="32"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>64</v>
       </c>
@@ -3936,7 +3901,7 @@
       <c r="L64" s="14"/>
       <c r="M64" s="15"/>
     </row>
-    <row r="65" spans="1:13" ht="12.75" customHeight="1">
+    <row r="65" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>65</v>
       </c>
@@ -3953,7 +3918,7 @@
       <c r="L65" s="17"/>
       <c r="M65" s="18"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>66</v>
       </c>
@@ -3970,7 +3935,7 @@
       <c r="L66" s="17"/>
       <c r="M66" s="18"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
         <v>67</v>
       </c>

</xml_diff>